<commit_message>
changed to digraph, updated functions
</commit_message>
<xml_diff>
--- a/cms_system_140.xlsx
+++ b/cms_system_140.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilkie/code/system_flow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{318BBFD7-F523-E747-8DB9-597FA40A7E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8957066-6CBD-E44C-B266-8D2BA50D77C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8140" yWindow="3380" windowWidth="16860" windowHeight="20720" activeTab="1" xr2:uid="{692BBBC8-C526-4D44-8BFB-29D6E6B2783D}"/>
+    <workbookView xWindow="26020" yWindow="6340" windowWidth="16860" windowHeight="20720" activeTab="1" xr2:uid="{692BBBC8-C526-4D44-8BFB-29D6E6B2783D}"/>
   </bookViews>
   <sheets>
     <sheet name="Detectors" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="39">
   <si>
     <t>Category</t>
   </si>
@@ -117,9 +117,6 @@
     <t>Muon RPC</t>
   </si>
   <si>
-    <t>Level-1 Trigger</t>
-  </si>
-  <si>
     <t>Inner Tracker</t>
   </si>
   <si>
@@ -147,7 +144,16 @@
     <t>Global</t>
   </si>
   <si>
-    <t>High-Level Trigger</t>
+    <t>Input</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Disk</t>
   </si>
 </sst>
 </file>
@@ -502,7 +508,7 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:J1"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -515,22 +521,22 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>32</v>
-      </c>
-      <c r="H1" t="s">
-        <v>33</v>
       </c>
       <c r="I1" t="s">
         <v>2</v>
@@ -544,7 +550,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2">
         <f>INT(1000000*J2)</f>
@@ -1192,102 +1198,230 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5BEB2EE-EDF9-134B-B756-B4F85E0E1D7D}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" t="s">
+        <v>2</v>
+      </c>
+      <c r="K1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
         <v>33</v>
       </c>
-      <c r="I1" t="s">
-        <v>2</v>
-      </c>
-      <c r="J1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
         <v>34</v>
       </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2">
-        <f>INT(1000000*J2)</f>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6">
+        <f>INT(1000000*K6)</f>
         <v>260000</v>
       </c>
-      <c r="D2">
+      <c r="E6">
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="F6">
         <v>400</v>
       </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
         <v>0.26</v>
       </c>
-      <c r="J2">
+      <c r="K6">
         <v>0.26</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="F7">
         <v>20</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating graph propagation methods
</commit_message>
<xml_diff>
--- a/cms_system_140.xlsx
+++ b/cms_system_140.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilkie/code/system_flow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8957066-6CBD-E44C-B266-8D2BA50D77C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DD5163-513B-F941-B1A8-50C573B4A5A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26020" yWindow="6340" windowWidth="16860" windowHeight="20720" activeTab="1" xr2:uid="{692BBBC8-C526-4D44-8BFB-29D6E6B2783D}"/>
+    <workbookView xWindow="27860" yWindow="5800" windowWidth="16860" windowHeight="20720" xr2:uid="{692BBBC8-C526-4D44-8BFB-29D6E6B2783D}"/>
   </bookViews>
   <sheets>
     <sheet name="Detectors" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
   <si>
     <t>Category</t>
   </si>
@@ -144,9 +144,6 @@
     <t>Global</t>
   </si>
   <si>
-    <t>Input</t>
-  </si>
-  <si>
     <t>Output</t>
   </si>
   <si>
@@ -154,6 +151,12 @@
   </si>
   <si>
     <t>Disk</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Sample Rate</t>
   </si>
 </sst>
 </file>
@@ -189,8 +192,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -505,15 +509,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55FF34C2-0233-224E-A21E-0372D088B6D7}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -524,28 +531,31 @@
         <v>27</v>
       </c>
       <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>30</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>31</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>32</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>2</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -554,14 +564,13 @@
       </c>
       <c r="C2">
         <f>INT(1000000*J2)</f>
-        <v>1440000</v>
-      </c>
-      <c r="D2">
-        <f>INT(40000000)</f>
+        <v>1010000</v>
+      </c>
+      <c r="D2" s="1">
         <v>40000000</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -573,13 +582,16 @@
         <v>0</v>
       </c>
       <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
         <v>1.01</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>1.44</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -588,14 +600,13 @@
       </c>
       <c r="C3">
         <f>INT(1000000*J3)</f>
-        <v>720000</v>
-      </c>
-      <c r="D3">
-        <f t="shared" ref="D3:D20" si="0">INT(40000000)</f>
+        <v>500000</v>
+      </c>
+      <c r="D3" s="1">
         <v>40000000</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -607,13 +618,16 @@
         <v>0</v>
       </c>
       <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
         <v>0.5</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>0.72</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -622,14 +636,13 @@
       </c>
       <c r="C4">
         <f>INT(1000000*J4)</f>
-        <v>430000</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="0"/>
+        <v>300000</v>
+      </c>
+      <c r="D4" s="1">
         <v>40000000</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -641,13 +654,16 @@
         <v>0</v>
       </c>
       <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
         <v>0.3</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>0.43</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -658,12 +674,11 @@
         <f>INT(1000000*J5)</f>
         <v>10000</v>
       </c>
-      <c r="D5">
-        <f t="shared" si="0"/>
+      <c r="D5" s="1">
         <v>40000000</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -675,13 +690,16 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -690,14 +708,13 @@
       </c>
       <c r="C6">
         <f>INT(1000000*J6)</f>
-        <v>240000</v>
-      </c>
-      <c r="D6">
-        <f t="shared" si="0"/>
+        <v>170000</v>
+      </c>
+      <c r="D6" s="1">
         <v>40000000</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -709,13 +726,16 @@
         <v>0</v>
       </c>
       <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
         <v>0.17</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>0.24</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -724,14 +744,13 @@
       </c>
       <c r="C7">
         <f>INT(1000000*J7)</f>
-        <v>440000</v>
-      </c>
-      <c r="D7">
-        <f t="shared" si="0"/>
+        <v>310000</v>
+      </c>
+      <c r="D7" s="1">
         <v>40000000</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -743,13 +762,16 @@
         <v>0</v>
       </c>
       <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
         <v>0.31</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>0.44</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -758,14 +780,13 @@
       </c>
       <c r="C8">
         <f>INT(1000000*J8)</f>
-        <v>600000</v>
-      </c>
-      <c r="D8">
-        <f t="shared" si="0"/>
+        <v>420000</v>
+      </c>
+      <c r="D8" s="1">
         <v>40000000</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -777,13 +798,16 @@
         <v>0</v>
       </c>
       <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
         <v>0.42</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>0.6</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -794,12 +818,11 @@
         <f>INT(1000000*J9)</f>
         <v>240000</v>
       </c>
-      <c r="D9">
-        <f t="shared" si="0"/>
+      <c r="D9" s="1">
         <v>40000000</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9">
         <v>0</v>
@@ -811,13 +834,16 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>0.24</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K9">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -828,12 +854,11 @@
         <f>INT(1000000*J10)</f>
         <v>30000</v>
       </c>
-      <c r="D10">
-        <f t="shared" si="0"/>
+      <c r="D10" s="1">
         <v>40000000</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10">
         <v>0</v>
@@ -845,13 +870,16 @@
         <v>0</v>
       </c>
       <c r="I10">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="J10">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K10">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -862,12 +890,11 @@
         <f>INT(1000000*J11)</f>
         <v>60000</v>
       </c>
-      <c r="D11">
-        <f t="shared" si="0"/>
+      <c r="D11" s="1">
         <v>40000000</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11">
         <v>0</v>
@@ -879,13 +906,16 @@
         <v>0</v>
       </c>
       <c r="I11">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="J11">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K11">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -894,14 +924,13 @@
       </c>
       <c r="C12">
         <f>INT(1000000*J12)</f>
-        <v>3000000</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
+        <v>2100000</v>
+      </c>
+      <c r="D12" s="1">
         <v>40000000</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F12">
         <v>0</v>
@@ -913,13 +942,16 @@
         <v>0</v>
       </c>
       <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
         <v>2.1</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -928,14 +960,13 @@
       </c>
       <c r="C13">
         <f>INT(1000000*J13)</f>
-        <v>150000</v>
-      </c>
-      <c r="D13">
-        <f t="shared" si="0"/>
+        <v>110000</v>
+      </c>
+      <c r="D13" s="1">
         <v>40000000</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F13">
         <v>0</v>
@@ -947,13 +978,16 @@
         <v>0</v>
       </c>
       <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
         <v>0.11</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>0.15</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -962,14 +996,13 @@
       </c>
       <c r="C14">
         <f>INT(1000000*J14)</f>
-        <v>50000</v>
-      </c>
-      <c r="D14">
-        <f t="shared" si="0"/>
+        <v>40000</v>
+      </c>
+      <c r="D14" s="1">
         <v>40000000</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14">
         <v>0</v>
@@ -981,13 +1014,16 @@
         <v>0</v>
       </c>
       <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
         <v>0.04</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>0.05</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -996,14 +1032,13 @@
       </c>
       <c r="C15">
         <f>INT(1000000*J15)</f>
-        <v>150000</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="0"/>
+        <v>110000</v>
+      </c>
+      <c r="D15" s="1">
         <v>40000000</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15">
         <v>0</v>
@@ -1015,13 +1050,16 @@
         <v>0</v>
       </c>
       <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
         <v>0.11</v>
       </c>
-      <c r="J15">
+      <c r="K15">
         <v>0.15</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1030,14 +1068,13 @@
       </c>
       <c r="C16">
         <f>INT(1000000*J16)</f>
-        <v>470000</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="0"/>
+        <v>330000</v>
+      </c>
+      <c r="D16" s="1">
         <v>40000000</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -1049,13 +1086,16 @@
         <v>0</v>
       </c>
       <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
         <v>0.33</v>
       </c>
-      <c r="J16">
+      <c r="K16">
         <v>0.47</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1064,14 +1104,13 @@
       </c>
       <c r="C17">
         <f>INT(1000000*J17)</f>
-        <v>3000</v>
-      </c>
-      <c r="D17">
-        <f t="shared" si="0"/>
+        <v>2000</v>
+      </c>
+      <c r="D17" s="1">
         <v>40000000</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -1083,13 +1122,16 @@
         <v>0</v>
       </c>
       <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
         <v>2E-3</v>
       </c>
-      <c r="J17">
+      <c r="K17">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1098,14 +1140,13 @@
       </c>
       <c r="C18">
         <f>INT(1000000*J18)</f>
-        <v>2000</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+      <c r="D18" s="1">
         <v>40000000</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F18">
         <v>0</v>
@@ -1117,13 +1158,16 @@
         <v>0</v>
       </c>
       <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
         <v>1E-3</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>2E-3</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1132,14 +1176,13 @@
       </c>
       <c r="C19">
         <f>INT(1000000*J19)</f>
-        <v>120000</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
+        <v>80000</v>
+      </c>
+      <c r="D19" s="1">
         <v>40000000</v>
       </c>
       <c r="E19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F19">
         <v>0</v>
@@ -1151,13 +1194,16 @@
         <v>0</v>
       </c>
       <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
         <v>0.08</v>
       </c>
-      <c r="J19">
+      <c r="K19">
         <v>0.12</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1168,12 +1214,11 @@
         <f>INT(1000000*J20)</f>
         <v>10000</v>
       </c>
-      <c r="D20">
-        <f t="shared" si="0"/>
+      <c r="D20" s="1">
         <v>40000000</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -1185,9 +1230,12 @@
         <v>0</v>
       </c>
       <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
         <v>0.01</v>
       </c>
-      <c r="J20">
+      <c r="K20">
         <v>0.01</v>
       </c>
     </row>
@@ -1198,10 +1246,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5BEB2EE-EDF9-134B-B756-B4F85E0E1D7D}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1209,7 +1257,7 @@
     <col min="1" max="1" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>35</v>
       </c>
@@ -1217,168 +1265,153 @@
         <v>36</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I1" t="s">
-        <v>32</v>
+        <v>2</v>
       </c>
       <c r="J1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>33</v>
       </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>33</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>33</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" t="s">
         <v>33</v>
       </c>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
+      <c r="C6">
+        <f>INT(1000000*J6)</f>
+        <v>260000</v>
       </c>
       <c r="D6">
-        <f>INT(1000000*K6)</f>
-        <v>260000</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>1</v>
+        <v>399</v>
       </c>
       <c r="F6">
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <v>0</v>
@@ -1387,41 +1420,61 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>0</v>
+        <v>0.26</v>
       </c>
       <c r="J6">
         <v>0.26</v>
       </c>
-      <c r="K6">
-        <v>0.26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
         <v>34</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>19</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>38</v>
       </c>
-      <c r="C7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7">
-        <v>20</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
moved prototypes to src file
</commit_message>
<xml_diff>
--- a/cms_system_140.xlsx
+++ b/cms_system_140.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilkie/code/system_flow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DD5163-513B-F941-B1A8-50C573B4A5A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193ED7A4-7240-3D4E-83E1-BFAD2A277D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="27860" yWindow="5800" windowWidth="16860" windowHeight="20720" xr2:uid="{692BBBC8-C526-4D44-8BFB-29D6E6B2783D}"/>
   </bookViews>
@@ -512,7 +512,7 @@
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
updating with new data and graph analytics
</commit_message>
<xml_diff>
--- a/cms_system_140.xlsx
+++ b/cms_system_140.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilkie/code/system_flow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193ED7A4-7240-3D4E-83E1-BFAD2A277D47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061E245E-16CE-AE42-A4A6-F2EA7F3FF909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27860" yWindow="5800" windowWidth="16860" windowHeight="20720" xr2:uid="{692BBBC8-C526-4D44-8BFB-29D6E6B2783D}"/>
+    <workbookView xWindow="2200" yWindow="5740" windowWidth="16920" windowHeight="20720" activeTab="1" xr2:uid="{692BBBC8-C526-4D44-8BFB-29D6E6B2783D}"/>
   </bookViews>
   <sheets>
     <sheet name="Detectors" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="40">
   <si>
     <t>Category</t>
   </si>
@@ -509,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55FF34C2-0233-224E-A21E-0372D088B6D7}">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -520,7 +520,7 @@
     <col min="2" max="2" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -551,11 +551,8 @@
       <c r="J1" t="s">
         <v>2</v>
       </c>
-      <c r="K1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -587,11 +584,8 @@
       <c r="J2">
         <v>1.01</v>
       </c>
-      <c r="K2">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -623,11 +617,8 @@
       <c r="J3">
         <v>0.5</v>
       </c>
-      <c r="K3">
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -659,11 +650,8 @@
       <c r="J4">
         <v>0.3</v>
       </c>
-      <c r="K4">
-        <v>0.43</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -695,11 +683,8 @@
       <c r="J5">
         <v>0.01</v>
       </c>
-      <c r="K5">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -731,11 +716,8 @@
       <c r="J6">
         <v>0.17</v>
       </c>
-      <c r="K6">
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -767,11 +749,8 @@
       <c r="J7">
         <v>0.31</v>
       </c>
-      <c r="K7">
-        <v>0.44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -803,11 +782,8 @@
       <c r="J8">
         <v>0.42</v>
       </c>
-      <c r="K8">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -839,11 +815,8 @@
       <c r="J9">
         <v>0.24</v>
       </c>
-      <c r="K9">
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -875,11 +848,8 @@
       <c r="J10">
         <v>0.03</v>
       </c>
-      <c r="K10">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -911,11 +881,8 @@
       <c r="J11">
         <v>0.06</v>
       </c>
-      <c r="K11">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -947,11 +914,8 @@
       <c r="J12">
         <v>2.1</v>
       </c>
-      <c r="K12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -983,11 +947,8 @@
       <c r="J13">
         <v>0.11</v>
       </c>
-      <c r="K13">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1019,11 +980,8 @@
       <c r="J14">
         <v>0.04</v>
       </c>
-      <c r="K14">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -1055,11 +1013,8 @@
       <c r="J15">
         <v>0.11</v>
       </c>
-      <c r="K15">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1091,11 +1046,8 @@
       <c r="J16">
         <v>0.33</v>
       </c>
-      <c r="K16">
-        <v>0.47</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1127,11 +1079,8 @@
       <c r="J17">
         <v>2E-3</v>
       </c>
-      <c r="K17">
-        <v>3.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -1163,11 +1112,8 @@
       <c r="J18">
         <v>1E-3</v>
       </c>
-      <c r="K18">
-        <v>2E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -1199,11 +1145,8 @@
       <c r="J19">
         <v>0.08</v>
       </c>
-      <c r="K19">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1233,9 +1176,6 @@
         <v>0</v>
       </c>
       <c r="J20">
-        <v>0.01</v>
-      </c>
-      <c r="K20">
         <v>0.01</v>
       </c>
     </row>
@@ -1248,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5BEB2EE-EDF9-134B-B756-B4F85E0E1D7D}">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
continuing refactor of power calculation
</commit_message>
<xml_diff>
--- a/cms_system_140.xlsx
+++ b/cms_system_140.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilkie/code/system_flow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1443656-2EFC-D24F-ABEF-E77603AED82C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF7772D-E566-4145-82C0-5A2EE812C31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11040" yWindow="3400" windowWidth="16920" windowHeight="20720" activeTab="1" xr2:uid="{692BBBC8-C526-4D44-8BFB-29D6E6B2783D}"/>
+    <workbookView xWindow="22180" yWindow="5800" windowWidth="20040" windowHeight="19960" xr2:uid="{692BBBC8-C526-4D44-8BFB-29D6E6B2783D}"/>
   </bookViews>
   <sheets>
     <sheet name="Detectors" sheetId="1" r:id="rId1"/>
     <sheet name="Triggers" sheetId="2" r:id="rId2"/>
+    <sheet name="Global" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
   <si>
     <t>Category</t>
   </si>
@@ -151,16 +152,32 @@
   </si>
   <si>
     <t>Skill variance</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Link Efficiency (J/bit)</t>
+  </si>
+  <si>
+    <t>Op Efficiency (J/op)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -186,9 +203,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,18 +521,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55FF34C2-0233-224E-A21E-0372D088B6D7}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="8" max="8" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -533,8 +552,14 @@
       <c r="F1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -554,8 +579,14 @@
       <c r="F2">
         <v>1.01</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="1">
+        <v>2.2200000000000002E-11</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -575,8 +606,14 @@
       <c r="F3">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="1">
+        <v>2.2200000000000002E-11</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -596,8 +633,14 @@
       <c r="F4">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="1">
+        <v>2.2200000000000002E-11</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -617,8 +660,14 @@
       <c r="F5">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="1">
+        <v>2.2200000000000002E-11</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -638,8 +687,14 @@
       <c r="F6">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="1">
+        <v>2.2200000000000002E-11</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -659,8 +714,14 @@
       <c r="F7">
         <v>0.31</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="1">
+        <v>2.2200000000000002E-11</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -680,8 +741,14 @@
       <c r="F8">
         <v>0.42</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="1">
+        <v>2.2200000000000002E-11</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -701,8 +768,14 @@
       <c r="F9">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G9" s="1">
+        <v>2.2200000000000002E-11</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -722,8 +795,14 @@
       <c r="F10">
         <v>0.03</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G10" s="1">
+        <v>2.2200000000000002E-11</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -743,8 +822,14 @@
       <c r="F11">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G11" s="1">
+        <v>2.2200000000000002E-11</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -764,8 +849,14 @@
       <c r="F12">
         <v>2.1</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G12" s="1">
+        <v>2.2200000000000002E-11</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -785,8 +876,14 @@
       <c r="F13">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G13" s="1">
+        <v>2.2200000000000002E-11</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -806,8 +903,14 @@
       <c r="F14">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G14" s="1">
+        <v>2.2200000000000002E-11</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -827,8 +930,14 @@
       <c r="F15">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G15" s="1">
+        <v>2.2200000000000002E-11</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -848,8 +957,14 @@
       <c r="F16">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G16" s="1">
+        <v>2.2200000000000002E-11</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -869,8 +984,14 @@
       <c r="F17">
         <v>2E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G17" s="1">
+        <v>2.2200000000000002E-11</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -890,8 +1011,14 @@
       <c r="F18">
         <v>1E-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G18" s="1">
+        <v>2.2200000000000002E-11</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -911,8 +1038,14 @@
       <c r="F19">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G19" s="1">
+        <v>2.2200000000000002E-11</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -931,6 +1064,12 @@
       </c>
       <c r="F20">
         <v>0.01</v>
+      </c>
+      <c r="G20" s="1">
+        <v>2.2200000000000002E-11</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -940,23 +1079,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5BEB2EE-EDF9-134B-B756-B4F85E0E1D7D}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
         <v>30</v>
-      </c>
-      <c r="B1" t="s">
-        <v>31</v>
       </c>
       <c r="C1" t="s">
         <v>26</v>
@@ -970,16 +1111,22 @@
       <c r="F1" t="s">
         <v>37</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>28</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -993,16 +1140,22 @@
       <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G2" s="1">
+        <v>2.5000000000000001E-11</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>28</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1016,16 +1169,22 @@
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G3" s="1">
+        <v>2.5000000000000001E-11</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
         <v>28</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1039,16 +1198,22 @@
       <c r="F4">
         <v>0</v>
       </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G4" s="1">
+        <v>2.5000000000000001E-11</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
         <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>18</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1062,16 +1227,22 @@
       <c r="F5">
         <v>0</v>
       </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G5" s="1">
+        <v>2.5000000000000001E-11</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" t="s">
         <v>29</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
       </c>
       <c r="C6">
         <v>260000</v>
@@ -1085,16 +1256,23 @@
       <c r="F6">
         <v>1</v>
       </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G6" s="1">
+        <v>2.5000000000000001E-11</v>
+      </c>
+      <c r="H6">
+        <f>120000/(40000000)</f>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" t="s">
         <v>32</v>
-      </c>
-      <c r="B7" t="s">
-        <v>29</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1108,16 +1286,23 @@
       <c r="F7">
         <v>1</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G7" s="1">
+        <v>2.5000000000000001E-11</v>
+      </c>
+      <c r="H7">
+        <f>1600000/(100000)</f>
+        <v>16</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" t="s">
         <v>33</v>
-      </c>
-      <c r="B8" t="s">
-        <v>32</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1131,8 +1316,39 @@
       <c r="F8">
         <v>0</v>
       </c>
-      <c r="G8">
-        <v>0</v>
+      <c r="G8" s="1">
+        <v>2.5000000000000001E-11</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADB14929-71FF-5B4E-ADBA-67CDD361E7BD}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>2028</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating and revising statistics propagation
</commit_message>
<xml_diff>
--- a/cms_system_140.xlsx
+++ b/cms_system_140.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilkie/code/system_flow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF7772D-E566-4145-82C0-5A2EE812C31E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AD329CF-B7B6-3747-8959-A9CB14930B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22180" yWindow="5800" windowWidth="20040" windowHeight="19960" xr2:uid="{692BBBC8-C526-4D44-8BFB-29D6E6B2783D}"/>
+    <workbookView xWindow="9900" yWindow="5740" windowWidth="20040" windowHeight="19960" activeTab="1" xr2:uid="{692BBBC8-C526-4D44-8BFB-29D6E6B2783D}"/>
   </bookViews>
   <sheets>
     <sheet name="Detectors" sheetId="1" r:id="rId1"/>
@@ -523,7 +523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55FF34C2-0233-224E-A21E-0372D088B6D7}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
@@ -1081,8 +1081,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5BEB2EE-EDF9-134B-B756-B4F85E0E1D7D}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1248,7 +1248,7 @@
         <v>260000</v>
       </c>
       <c r="D6">
-        <v>400</v>
+        <v>80</v>
       </c>
       <c r="E6">
         <v>3</v>
@@ -1278,7 +1278,7 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="E7">
         <v>4</v>

</xml_diff>

<commit_message>
updating spreadsheet to resolve colab error
</commit_message>
<xml_diff>
--- a/cms_system_140.xlsx
+++ b/cms_system_140.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilkie/code/system_flow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4D6F94-902B-984A-B72E-B30F3947308F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771F0989-67BE-0742-A524-9490CF54AB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="26360" yWindow="2540" windowWidth="20040" windowHeight="19960" activeTab="1" xr2:uid="{692BBBC8-C526-4D44-8BFB-29D6E6B2783D}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="40">
   <si>
     <t>Category</t>
   </si>
@@ -137,9 +137,6 @@
   </si>
   <si>
     <t>Disk</t>
-  </si>
-  <si>
-    <t>None</t>
   </si>
   <si>
     <t>Sample Rate</t>
@@ -544,16 +541,16 @@
         <v>26</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
         <v>27</v>
       </c>
       <c r="F1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G1" t="s">
         <v>39</v>
-      </c>
-      <c r="G1" t="s">
-        <v>40</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
@@ -567,7 +564,7 @@
         <v>25</v>
       </c>
       <c r="C2">
-        <f>INT(1000000*H2)</f>
+        <f t="shared" ref="C2:C20" si="0">INT(1000000*H2)</f>
         <v>1010000</v>
       </c>
       <c r="D2" s="1">
@@ -594,7 +591,7 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <f>INT(1000000*H3)</f>
+        <f t="shared" si="0"/>
         <v>500000</v>
       </c>
       <c r="D3" s="1">
@@ -621,7 +618,7 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <f>INT(1000000*H4)</f>
+        <f t="shared" si="0"/>
         <v>300000</v>
       </c>
       <c r="D4" s="1">
@@ -648,7 +645,7 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <f>INT(1000000*H5)</f>
+        <f t="shared" si="0"/>
         <v>10000</v>
       </c>
       <c r="D5" s="1">
@@ -675,7 +672,7 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <f>INT(1000000*H6)</f>
+        <f t="shared" si="0"/>
         <v>170000</v>
       </c>
       <c r="D6" s="1">
@@ -702,7 +699,7 @@
         <v>9</v>
       </c>
       <c r="C7">
-        <f>INT(1000000*H7)</f>
+        <f t="shared" si="0"/>
         <v>310000</v>
       </c>
       <c r="D7" s="1">
@@ -729,7 +726,7 @@
         <v>11</v>
       </c>
       <c r="C8">
-        <f>INT(1000000*H8)</f>
+        <f t="shared" si="0"/>
         <v>420000</v>
       </c>
       <c r="D8" s="1">
@@ -756,7 +753,7 @@
         <v>12</v>
       </c>
       <c r="C9">
-        <f>INT(1000000*H9)</f>
+        <f t="shared" si="0"/>
         <v>240000</v>
       </c>
       <c r="D9" s="1">
@@ -783,7 +780,7 @@
         <v>13</v>
       </c>
       <c r="C10">
-        <f>INT(1000000*H10)</f>
+        <f t="shared" si="0"/>
         <v>30000</v>
       </c>
       <c r="D10" s="1">
@@ -810,7 +807,7 @@
         <v>14</v>
       </c>
       <c r="C11">
-        <f>INT(1000000*H11)</f>
+        <f t="shared" si="0"/>
         <v>60000</v>
       </c>
       <c r="D11" s="1">
@@ -837,7 +834,7 @@
         <v>15</v>
       </c>
       <c r="C12">
-        <f>INT(1000000*H12)</f>
+        <f t="shared" si="0"/>
         <v>2100000</v>
       </c>
       <c r="D12" s="1">
@@ -864,7 +861,7 @@
         <v>16</v>
       </c>
       <c r="C13">
-        <f>INT(1000000*H13)</f>
+        <f t="shared" si="0"/>
         <v>110000</v>
       </c>
       <c r="D13" s="1">
@@ -891,7 +888,7 @@
         <v>17</v>
       </c>
       <c r="C14">
-        <f>INT(1000000*H14)</f>
+        <f t="shared" si="0"/>
         <v>40000</v>
       </c>
       <c r="D14" s="1">
@@ -918,7 +915,7 @@
         <v>19</v>
       </c>
       <c r="C15">
-        <f>INT(1000000*H15)</f>
+        <f t="shared" si="0"/>
         <v>110000</v>
       </c>
       <c r="D15" s="1">
@@ -945,7 +942,7 @@
         <v>20</v>
       </c>
       <c r="C16">
-        <f>INT(1000000*H16)</f>
+        <f t="shared" si="0"/>
         <v>330000</v>
       </c>
       <c r="D16" s="1">
@@ -972,7 +969,7 @@
         <v>21</v>
       </c>
       <c r="C17">
-        <f>INT(1000000*H17)</f>
+        <f t="shared" si="0"/>
         <v>2000</v>
       </c>
       <c r="D17" s="1">
@@ -999,7 +996,7 @@
         <v>22</v>
       </c>
       <c r="C18">
-        <f>INT(1000000*H18)</f>
+        <f t="shared" si="0"/>
         <v>1000</v>
       </c>
       <c r="D18" s="1">
@@ -1026,7 +1023,7 @@
         <v>23</v>
       </c>
       <c r="C19">
-        <f>INT(1000000*H19)</f>
+        <f t="shared" si="0"/>
         <v>80000</v>
       </c>
       <c r="D19" s="1">
@@ -1053,7 +1050,7 @@
         <v>24</v>
       </c>
       <c r="C20">
-        <f>INT(1000000*H20)</f>
+        <f t="shared" si="0"/>
         <v>10000</v>
       </c>
       <c r="D20" s="1">
@@ -1082,7 +1079,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1103,19 +1100,19 @@
         <v>26</v>
       </c>
       <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>36</v>
       </c>
-      <c r="F1" t="s">
-        <v>37</v>
-      </c>
       <c r="G1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="I1" t="s">
         <v>27</v>
@@ -1300,9 +1297,6 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>32</v>
-      </c>
-      <c r="B8" t="s">
-        <v>33</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1343,7 +1337,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
refactoring "triggers" as "processors"
</commit_message>
<xml_diff>
--- a/cms_system_140.xlsx
+++ b/cms_system_140.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wilkie/code/system_flow/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{771F0989-67BE-0742-A524-9490CF54AB71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB571512-92BA-1A49-B480-787E74AFA140}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26360" yWindow="2540" windowWidth="20040" windowHeight="19960" activeTab="1" xr2:uid="{692BBBC8-C526-4D44-8BFB-29D6E6B2783D}"/>
+    <workbookView xWindow="13860" yWindow="2260" windowWidth="25000" windowHeight="21180" activeTab="1" xr2:uid="{692BBBC8-C526-4D44-8BFB-29D6E6B2783D}"/>
   </bookViews>
   <sheets>
     <sheet name="Detectors" sheetId="1" r:id="rId1"/>
-    <sheet name="Triggers" sheetId="2" r:id="rId2"/>
+    <sheet name="Processors" sheetId="2" r:id="rId2"/>
     <sheet name="Global" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -222,9 +222,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -262,7 +262,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -368,7 +368,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -510,7 +510,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1079,7 +1079,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>